<commit_message>
Make fancier antibodies submission XLSX file
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -4,10 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Antibodies" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Antibodies" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Terminology" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -78,14 +80,29 @@
         <t>Missing required value 'Antibody name'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B3" shapeId="0">
+    <comment authorId="0" ref="B5" shapeId="0">
       <text>
-        <t>'Martian' is not regognized host</t>
+        <t>Missing required value 'Host'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C3" shapeId="0">
+    <comment authorId="0" ref="B6" shapeId="0">
       <text>
-        <t>Missing required value 'Isoform'</t>
+        <t>'Mu musculus' is not a recognized host</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B7" shapeId="0">
+      <text>
+        <t>'Coronavirus' is not a recognized host</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C9" shapeId="0">
+      <text>
+        <t>Missing required value 'Isotype'</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C10" shapeId="0">
+      <text>
+        <t>'Ig' is not a recognized isotype</t>
       </text>
     </comment>
   </commentList>
@@ -376,16 +393,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CoVIC-DB Antibodies Submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Add your antibodies to the 'Antibodies' sheet. Do not edit the other sheets.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Columns:</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>- Antibody name: Your institutions preferred name for the antibody.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>- Host: The name of the host species that is the source of the antibody.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>- Isotype: The name of the isotype of the antibody's heavy chain.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -408,7 +493,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Isoform</t>
+          <t>Isotype</t>
         </is>
       </c>
     </row>
@@ -425,21 +510,326 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>foo</t>
+          <t>IgA</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr"/>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Martian</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>IgD</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Acme mAb 3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Mus musculus</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>IgG</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Acme mAb 4</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>IgG2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Acme mAb 5</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Mu musculus</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>IgA1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Acme mAb 6</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Coronavirus</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>IgA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Acme mAb 7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>IgE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Acme mAb 8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mus musculus</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Acme mAb 9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Acme mAb 10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mus musculus</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>IgM</t>
+        </is>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B100" type="list">
+      <formula1>=Terminology!A2:A3</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C100" type="list">
+      <formula1>=Terminology!B2:B16</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="15"/>
+    <col customWidth="1" max="2" min="2" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Isotype</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>IgA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mus musculus</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IgA1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>IgA2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>IgD</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>IgE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IgG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>IgG1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IgG2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IgG2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>IgG2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>IgG2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>IgG3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>IgG4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IgM</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sIgA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Do not allow duplicate antibody names
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -80,27 +80,32 @@
         <t>Missing required value 'Antibody name'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B5" shapeId="0">
+    <comment authorId="0" ref="A4" shapeId="0">
+      <text>
+        <t>Duplicate antibody name 'Acme mAb 1' is not allowed</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B6" shapeId="0">
       <text>
         <t>Missing required value 'Host'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B6" shapeId="0">
+    <comment authorId="0" ref="B7" shapeId="0">
       <text>
         <t>'Mu musculus' is not a recognized host</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B7" shapeId="0">
+    <comment authorId="0" ref="B8" shapeId="0">
       <text>
         <t>'Coronavirus' is not a recognized host</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C9" shapeId="0">
+    <comment authorId="0" ref="C10" shapeId="0">
       <text>
         <t>Missing required value 'Isotype'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C10" shapeId="0">
+    <comment authorId="0" ref="C11" shapeId="0">
       <text>
         <t>'Ig' is not a recognized isotype</t>
       </text>
@@ -528,9 +533,9 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Acme mAb 3</t>
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Acme mAb 1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -550,7 +555,11 @@
           <t>Acme mAb 4</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>IgG2a</t>
@@ -563,11 +572,7 @@
           <t>Acme mAb 5</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Mu musculus</t>
-        </is>
-      </c>
+      <c r="B6" s="2" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>IgA1</t>
@@ -582,7 +587,7 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Coronavirus</t>
+          <t>Mu musculus</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -597,9 +602,9 @@
           <t>Acme mAb 7</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Homo sapiens</t>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Coronavirus</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -619,7 +624,11 @@
           <t>Mus musculus</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>IgA2</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -632,11 +641,7 @@
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>Ig</t>
-        </is>
-      </c>
+      <c r="C10" s="2" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -649,9 +654,9 @@
           <t>Mus musculus</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>IgM</t>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Ig</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Rework ontology templates and reuse them better
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -663,7 +663,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B100" type="list">
-      <formula1>=Terminology!A2:A3</formula1>
+      <formula1>=Terminology!A2:A4</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C100" type="list">
       <formula1>=Terminology!B2:B16</formula1>
@@ -730,7 +730,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mus musculus BALB/C</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>IgA2</t>

</xml_diff>

<commit_message>
Add examples and validation for first assay type
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -441,7 +441,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>- Antibody name: Your institutions preferred name for the antibody.</t>
+          <t>- Antibody name: Your institution's preferred name for the antibody.</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       <formula1>=Terminology!A2:A4</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C100" type="list">
-      <formula1>=Terminology!B2:B16</formula1>
+      <formula1>=Terminology!B2:B17</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -680,7 +680,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -833,7 +833,15 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>sIgA</t>
+          <t>kappa</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>lambda</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix formulas for data validations
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -663,10 +663,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B100" type="list">
-      <formula1>=Terminology!A2:A4</formula1>
+      <formula1>=Terminology!$A$2:$A$4</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C100" type="list">
-      <formula1>=Terminology!B2:B17</formula1>
+      <formula1>=Terminology!$B$2:$B$17</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Add sumbissions module, refactor, revise examples
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -75,39 +75,34 @@
     <author>Validation service</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3" shapeId="0">
-      <text>
-        <t>Missing required value 'Antibody name'</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="A4" shapeId="0">
       <text>
-        <t>Duplicate antibody name 'Acme mAb 1' is not allowed</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B6" shapeId="0">
-      <text>
-        <t>Missing required value 'Host'</t>
+        <t>Missing required value for 'Antibody name'</t>
       </text>
     </comment>
     <comment authorId="0" ref="B7" shapeId="0">
       <text>
-        <t>'Mu musculus' is not a recognized host</t>
+        <t>Missing required value for 'Host'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B8" shapeId="0">
+    <comment authorId="0" ref="C7" shapeId="0">
       <text>
-        <t>'Coronavirus' is not a recognized host</t>
+        <t>'Ig1' is not a recognized value for 'Isotype'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C10" shapeId="0">
+    <comment authorId="0" ref="B9" shapeId="0">
       <text>
-        <t>Missing required value 'Isotype'</t>
+        <t>'Mus musclus' is not a recognized value for 'Host'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C11" shapeId="0">
+    <comment authorId="0" ref="C9" shapeId="0">
       <text>
-        <t>'Ig' is not a recognized isotype</t>
+        <t>'Igm' is not a recognized value for 'Isotype'</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A10" shapeId="0">
+      <text>
+        <t>Duplicate value 'C3' is not allowed for 'Antibody name'</t>
       </text>
     </comment>
   </commentList>
@@ -471,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -505,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Acme mAb 1</t>
+          <t>A6</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -520,10 +515,14 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>B12</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Mus musculus</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,11 +532,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Acme mAb 1</t>
-        </is>
-      </c>
+      <c r="A4" s="2" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
           <t>Mus musculus</t>
@@ -545,66 +540,66 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IgG</t>
+          <t>IgD</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Acme mAb 4</t>
+          <t>C2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Mus musculus</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IgG2a</t>
+          <t>IgG</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Acme mAb 5</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr"/>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>IgA1</t>
+          <t>IgG2a</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Acme mAb 6</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>Mu musculus</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>IgA</t>
+          <t>C6</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr"/>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Ig1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Acme mAb 7</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Coronavirus</t>
+          <t>D12</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -616,24 +611,24 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Acme mAb 8</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Mus musculus</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>IgA2</t>
+          <t>E8</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Mus musclus</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Igm</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Acme mAb 9</t>
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>C3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -641,22 +636,9 @@
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Acme mAb 10</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Mus musculus</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>Ig</t>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>IgG2a</t>
         </is>
       </c>
     </row>
@@ -666,7 +648,7 @@
       <formula1>=Terminology!$A$2:$A$4</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C100" type="list">
-      <formula1>=Terminology!$B$2:$B$17</formula1>
+      <formula1>=Terminology!$B$2:$B$15</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -680,7 +662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -829,22 +811,6 @@
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>kappa</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>lambda</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Add columns to antibodies table
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -398,7 +398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,20 @@
       <c r="A8" t="inlineStr">
         <is>
           <t>- Isotype: The name of the isotype of the antibody's heavy chain.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>- Antibody details: Measurements or characteristics of the antibody</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>- Antibody comment: Other comments on the antibody</t>
         </is>
       </c>
     </row>
@@ -466,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -478,6 +492,8 @@
     <col customWidth="1" max="1" min="1" width="15"/>
     <col customWidth="1" max="2" min="2" width="15"/>
     <col customWidth="1" max="3" min="3" width="15"/>
+    <col customWidth="1" max="4" min="4" width="16"/>
+    <col customWidth="1" max="5" min="5" width="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -496,6 +512,16 @@
           <t>Isotype</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Antibody details</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Antibody comment</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -513,6 +539,8 @@
           <t>IgA</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -530,6 +558,8 @@
           <t>IgD</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr"/>
@@ -543,6 +573,8 @@
           <t>IgD</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -560,6 +592,8 @@
           <t>IgG</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -577,6 +611,8 @@
           <t>IgG2a</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -590,6 +626,8 @@
           <t>Ig1</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -607,6 +645,8 @@
           <t>IgE</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -624,6 +664,8 @@
           <t>Igm</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
@@ -641,6 +683,8 @@
           <t>IgG2a</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Switch to more complex SPR example
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -77,32 +77,32 @@
   <commentList>
     <comment authorId="0" ref="A4" shapeId="0">
       <text>
-        <t>Missing required value for 'Antibody name'</t>
+        <t>Missing required value in column 'Antibody name'</t>
       </text>
     </comment>
     <comment authorId="0" ref="B7" shapeId="0">
       <text>
-        <t>Missing required value for 'Host'</t>
+        <t>Missing required value in column 'Host'</t>
       </text>
     </comment>
     <comment authorId="0" ref="C7" shapeId="0">
       <text>
-        <t>'Ig1' is not a recognized value for 'Isotype'</t>
+        <t>'Ig1' is not a valid term in column 'Isotype'</t>
       </text>
     </comment>
     <comment authorId="0" ref="B9" shapeId="0">
       <text>
-        <t>'Mus musclus' is not a recognized value for 'Host'</t>
+        <t>'Mus musclus' is not a valid term in column 'Host'</t>
       </text>
     </comment>
     <comment authorId="0" ref="C9" shapeId="0">
       <text>
-        <t>'Igm' is not a recognized value for 'Isotype'</t>
+        <t>'Igm' is not a valid term in column 'Isotype'</t>
       </text>
     </comment>
     <comment authorId="0" ref="A10" shapeId="0">
       <text>
-        <t>Duplicate value 'C3' is not allowed for 'Antibody name'</t>
+        <t>Duplicate value 'C3' is not allowed in column 'Antibody name'</t>
       </text>
     </comment>
   </commentList>

</xml_diff>

<commit_message>
Revise antibody template 1.2
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -75,34 +75,39 @@
     <author>Validation service</author>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A3" shapeId="0">
+      <text>
+        <t>Duplicate value 'VD-Crotty 1' is not allowed in column 'Antibody name'</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="A4" shapeId="0">
       <text>
         <t>Missing required value in column 'Antibody name'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B7" shapeId="0">
+    <comment authorId="0" ref="B5" shapeId="0">
       <text>
         <t>Missing required value in column 'Host'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C7" shapeId="0">
+    <comment authorId="0" ref="C6" shapeId="0">
       <text>
-        <t>'Ig1' is not a valid term in column 'Isotype'</t>
+        <t>'IggA1' is not a valid term in column 'Isotype'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B9" shapeId="0">
+    <comment authorId="0" ref="D7" shapeId="0">
       <text>
-        <t>'Mus musclus' is not a valid term in column 'Host'</t>
+        <t>'kapa' is not a valid term in column 'Light chain'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C9" shapeId="0">
+    <comment authorId="0" ref="E8" shapeId="0">
       <text>
-        <t>'Igm' is not a valid term in column 'Isotype'</t>
+        <t>'IGVH1-8' is not a valid term in column 'Heavy chain germline'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A10" shapeId="0">
+    <comment authorId="0" ref="G9" shapeId="0">
       <text>
-        <t>Duplicate value 'C3' is not allowed in column 'Antibody name'</t>
+        <t>'top' is not of type 'integer' in column 'Structural data'</t>
       </text>
     </comment>
   </commentList>
@@ -398,13 +403,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="18"/>
+    <col customWidth="1" max="2" min="2" width="70"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -412,59 +421,190 @@
           <t>CoVIC-DB Antibodies Submission</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Version 1.2</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Add your antibodies to the 'Antibodies' sheet. Do not edit the other sheets.</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Columns:</t>
-        </is>
-      </c>
-    </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>- Antibody name: Your preferred code name for the antibody.</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Antibody name</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Your preferred code name for the antibody</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>- Host: The name of the host species that is the source of the antibody.</t>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Specify the host species that is the source of the antibody</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>- Isotype: The name of the isotype of the antibody's heavy chain.</t>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Isotype</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Specify the antibody isotype, if known</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>- Antibody details: Measurements or characteristics of the antibody</t>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Light chain</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Specify the antibody light chain, if known (kappa or lambda)</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>- Antibody comment: Other comments on the antibody</t>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Heavy chain germline</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Specify the antibody heavy chain germline gene, if known</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Antibody details</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Measurements or characteristics of the antibody.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>This column is optional, and meant to capture data you might have on the antibody.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>These data will not be released to the partner reference labs that will perform the analyses.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>For example:</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- Affinity: Spike protein binding affinity; inhibition of ACE2 binding; ELISA for Spike </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>- Neutralization: IC50 value</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>- Neutralization assay platform</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>- Epitope: Binning or competition data</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Structural data</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Would you like structural analyses of this antibody?</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>If no, leave blank.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>If yes, rank the antibodies in order of priority, starting with '1' for the highest priority.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Antibody comment</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Please provide any other details about the antibody.</t>
         </is>
       </c>
     </row>
@@ -480,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -492,8 +632,11 @@
     <col customWidth="1" max="1" min="1" width="15"/>
     <col customWidth="1" max="2" min="2" width="15"/>
     <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="16"/>
-    <col customWidth="1" max="5" min="5" width="16"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
+    <col customWidth="1" max="6" min="6" width="16"/>
+    <col customWidth="1" max="7" min="7" width="15"/>
+    <col customWidth="1" max="8" min="8" width="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -514,10 +657,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Light chain</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Heavy chain germline</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Antibody details</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Structural data</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Antibody comment</t>
         </is>
@@ -526,7 +684,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A6</t>
+          <t>VD-Crotty 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -539,18 +697,33 @@
           <t>IgA</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>kappa</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>IGHV1-8</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Spike protein binding affinity</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>B12</t>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>VD-Crotty 1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mus musculus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -558,8 +731,27 @@
           <t>IgD</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>lambda</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>IGHV1-18</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>inhibition of ACE2 binding</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr"/>
@@ -570,69 +762,129 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IgD</t>
+          <t>IgG</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>IGHV2-5</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ELISA for Spike</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Mus musculus</t>
-        </is>
-      </c>
+          <t>VD-Crotty 4</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IgG</t>
+          <t>IgG2a</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>IGHV3-7</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>IC50 value</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>VD-Crotty 5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>IgG2a</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+          <t>Mus musculus</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>IggA1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>kappa</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>IGHV3-11</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Neutralization assay platform</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>A comment</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C6</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr"/>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>Ig1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>VD-Crotty 6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mus musculus</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>IgA</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>kapa</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Epitope binning data</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>D12</t>
+          <t>VD-Crotty 7</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -646,31 +898,61 @@
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>IGVH1-8</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Epitope competition data</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>E8</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>Mus musclus</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>Igm</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>VD-Crotty 8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mus musculus</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>IgA2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>lambda</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>top</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Another comment</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>C3</t>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>VD-Crotty 9</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -680,19 +962,54 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>IgG2a</t>
+          <t>IgG1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>VD-Crotty 10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mus musculus</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>IgM</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="4">
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B100" type="list">
       <formula1>=Terminology!$A$2:$A$4</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C100" type="list">
       <formula1>=Terminology!$B$2:$B$15</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D100" type="list">
+      <formula1>=Terminology!$C$2:$C$3</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E100" type="list">
+      <formula1>=Terminology!$D$2:$D$12</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -706,7 +1023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -717,6 +1034,8 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="15"/>
     <col customWidth="1" max="2" min="2" width="15"/>
+    <col customWidth="1" max="3" min="3" width="15"/>
+    <col customWidth="1" max="4" min="4" width="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -730,6 +1049,16 @@
           <t>Isotype</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Light chain</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Heavy chain germline</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -742,6 +1071,16 @@
           <t>IgA</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>kappa</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>IGHV1-8</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -754,6 +1093,16 @@
           <t>IgA1</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>lambda</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>IGHV1-18</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -764,6 +1113,12 @@
       <c r="B4" t="inlineStr">
         <is>
           <t>IgA2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>IGHV2-5</t>
         </is>
       </c>
     </row>
@@ -774,6 +1129,12 @@
           <t>IgD</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>IGHV3-7</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -782,6 +1143,12 @@
           <t>IgE</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>IGHV3-11</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -790,6 +1157,12 @@
           <t>IgG</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>IGHV3-21</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -798,6 +1171,12 @@
           <t>IgG1</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>IGHV3-23</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -806,6 +1185,12 @@
           <t>IgG2</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>IGHV4-39</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -814,6 +1199,12 @@
           <t>IgG2a</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>IGHV4-59</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -822,6 +1213,12 @@
           <t>IgG2b</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>IGHV5-51</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -830,6 +1227,12 @@
           <t>IgG2c</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>IGHV6-1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -838,6 +1241,8 @@
           <t>IgG3</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -846,6 +1251,8 @@
           <t>IgG4</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -854,6 +1261,8 @@
           <t>IgM</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
     </row>
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>

</xml_diff>

<commit_message>
Add more heavy chains
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -426,7 +426,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Version 1.2</t>
+          <t>Version 1.2.1</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       <formula1>=Terminology!$C$2:$C$3</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E100" type="list">
-      <formula1>=Terminology!$D$2:$D$12</formula1>
+      <formula1>=Terminology!$D$2:$D$136</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1023,7 +1023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>IGHV1-8</t>
+          <t>IGHA1</t>
         </is>
       </c>
     </row>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>IGHV1-18</t>
+          <t>IGHA2</t>
         </is>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>IGHV2-5</t>
+          <t>IGHD</t>
         </is>
       </c>
     </row>
@@ -1132,7 +1132,7 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>IGHV3-7</t>
+          <t>IGHD1-1</t>
         </is>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>IGHV3-11</t>
+          <t>IGHE</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>IGHV3-21</t>
+          <t>IGHG1</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>IGHV3-23</t>
+          <t>IGHG2</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>IGHV4-39</t>
+          <t>IGHG3</t>
         </is>
       </c>
     </row>
@@ -1202,7 +1202,7 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>IGHV4-59</t>
+          <t>IGHG4</t>
         </is>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>IGHV5-51</t>
+          <t>IGHJ1</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1230,7 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>IGHV6-1</t>
+          <t>IGHM</t>
         </is>
       </c>
     </row>
@@ -1242,7 +1242,11 @@
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>IGHV1-18</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -1252,7 +1256,11 @@
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>IGHV1-2</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -1262,7 +1270,1221 @@
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>IGHV1-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>IGHV1-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>IGHV1-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>IGHV1-46</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>IGHV1-58</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>IGHV1-69</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>IGHV1-69-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>IGHV1-69D</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>IGHV1-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>IGHV2-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>IGHV2-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>IGHV2-70</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>IGHV3-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>IGHV3-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>IGHV3-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>IGHV3-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>IGHV3-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>IGHV3-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>IGHV3-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>IGHV3-30-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>IGHV3-30-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>IGHV3-33</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>IGHV3-43</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>IGHV3-43D</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>IGHV3-48</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>IGHV3-49</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>IGHV3-53</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>IGHV3-64</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>IGHV3-66</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>IGHV3-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>IGHV3-72</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>IGHV3-73</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>IGHV3-74</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>IGHV3-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>IGHV4-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>IGHV4-30-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>IGHV4-30-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>IGHV4-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>IGHV4-34</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>IGHV4-38-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>IGHV4-39</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>IGHV4-4</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>IGHV4-59</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>IGHV4-61</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>IGHV5-10-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>IGHV5-51</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>IGHV6-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>IGHV7-4-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>IGKJ1</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>IGKV1-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>IGKV1-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>IGKV1-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>IGKV1-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>IGKV1-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>IGKV1-33</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>IGKV1-39</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>IGKV1-5</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>IGKV1-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>IGKV1-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>IGKV1-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>IGKV1D-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>IGKV1D-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>IGKV1D-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>IGKV1D-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>IGKV1D-33</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>IGKV1D-39</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>IGKV1D-43</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>IGKV1D-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>IGKV2-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>IGKV2-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>IGKV2-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>IGKV2-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>IGKV2-40</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>IGKV2D-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>IGKV2D-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>IGKV2D-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>IGKV2D-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>IGKV2D-40</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>IGKV3-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>IGKV3-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>IGKV3-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>IGKV3D-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>IGKV3D-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>IGKV3D-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>IGKV3D-7</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>IGKV4-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>IGKV5-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>IGKV6-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>IGKV6D-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>IGLJ1</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>IGLV1-36</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>IGLV1-40</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>IGLV1-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>IGLV1-47</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>IGLV1-51</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>IGLV10-54</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>IGLV2-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>IGLV2-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>IGLV2-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>IGLV2-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>IGLV2-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>IGLV3-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>IGLV3-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr"/>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>IGLV3-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>IGLV3-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>IGLV3-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>IGLV3-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>IGLV3-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>IGLV3-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>IGLV3-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>IGLV4-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr"/>
+      <c r="B126" t="inlineStr"/>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>IGLV4-60</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>IGLV4-69</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr"/>
+      <c r="B128" t="inlineStr"/>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>IGLV5-37</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>IGLV5-39</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr"/>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>IGLV5-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr"/>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>IGLV5-52</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr"/>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>IGLV6-57</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr"/>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>IGLV7-43</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr"/>
+      <c r="B134" t="inlineStr"/>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>IGLV7-46</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>IGLV8-61</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr"/>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>IGLV9-49</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>

</xml_diff>

<commit_message>
Limit heavy chains to IGHV
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -1009,7 +1009,7 @@
       <formula1>=Terminology!$C$2:$C$3</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E100" type="list">
-      <formula1>=Terminology!$D$2:$D$136</formula1>
+      <formula1>=Terminology!$D$2:$D$51</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1023,7 +1023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>IGHA1</t>
+          <t>IGHV1-18</t>
         </is>
       </c>
     </row>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>IGHA2</t>
+          <t>IGHV1-2</t>
         </is>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>IGHD</t>
+          <t>IGHV1-24</t>
         </is>
       </c>
     </row>
@@ -1132,7 +1132,7 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>IGHD1-1</t>
+          <t>IGHV1-3</t>
         </is>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>IGHE</t>
+          <t>IGHV1-45</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>IGHG1</t>
+          <t>IGHV1-46</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>IGHG2</t>
+          <t>IGHV1-58</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>IGHG3</t>
+          <t>IGHV1-69</t>
         </is>
       </c>
     </row>
@@ -1202,7 +1202,7 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>IGHG4</t>
+          <t>IGHV1-69-2</t>
         </is>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>IGHJ1</t>
+          <t>IGHV1-69D</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1230,7 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>IGHM</t>
+          <t>IGHV1-8</t>
         </is>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>IGHV1-18</t>
+          <t>IGHV2-26</t>
         </is>
       </c>
     </row>
@@ -1258,7 +1258,7 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>IGHV1-2</t>
+          <t>IGHV2-5</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>IGHV1-24</t>
+          <t>IGHV2-70</t>
         </is>
       </c>
     </row>
@@ -1282,7 +1282,7 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>IGHV1-3</t>
+          <t>IGHV3-11</t>
         </is>
       </c>
     </row>
@@ -1292,7 +1292,7 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>IGHV1-45</t>
+          <t>IGHV3-13</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>IGHV1-46</t>
+          <t>IGHV3-15</t>
         </is>
       </c>
     </row>
@@ -1312,7 +1312,7 @@
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>IGHV1-58</t>
+          <t>IGHV3-20</t>
         </is>
       </c>
     </row>
@@ -1322,7 +1322,7 @@
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>IGHV1-69</t>
+          <t>IGHV3-21</t>
         </is>
       </c>
     </row>
@@ -1332,7 +1332,7 @@
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>IGHV1-69-2</t>
+          <t>IGHV3-23</t>
         </is>
       </c>
     </row>
@@ -1342,7 +1342,7 @@
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>IGHV1-69D</t>
+          <t>IGHV3-30</t>
         </is>
       </c>
     </row>
@@ -1352,7 +1352,7 @@
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>IGHV1-8</t>
+          <t>IGHV3-30-3</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1362,7 @@
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>IGHV2-26</t>
+          <t>IGHV3-30-5</t>
         </is>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>IGHV2-5</t>
+          <t>IGHV3-33</t>
         </is>
       </c>
     </row>
@@ -1382,7 +1382,7 @@
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>IGHV2-70</t>
+          <t>IGHV3-43</t>
         </is>
       </c>
     </row>
@@ -1392,7 +1392,7 @@
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>IGHV3-11</t>
+          <t>IGHV3-43D</t>
         </is>
       </c>
     </row>
@@ -1402,7 +1402,7 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>IGHV3-13</t>
+          <t>IGHV3-48</t>
         </is>
       </c>
     </row>
@@ -1412,7 +1412,7 @@
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>IGHV3-15</t>
+          <t>IGHV3-49</t>
         </is>
       </c>
     </row>
@@ -1422,7 +1422,7 @@
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>IGHV3-20</t>
+          <t>IGHV3-53</t>
         </is>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>IGHV3-21</t>
+          <t>IGHV3-64</t>
         </is>
       </c>
     </row>
@@ -1442,7 +1442,7 @@
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>IGHV3-23</t>
+          <t>IGHV3-66</t>
         </is>
       </c>
     </row>
@@ -1452,7 +1452,7 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>IGHV3-30</t>
+          <t>IGHV3-7</t>
         </is>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr">
         <is>
-          <t>IGHV3-30-3</t>
+          <t>IGHV3-72</t>
         </is>
       </c>
     </row>
@@ -1472,7 +1472,7 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr">
         <is>
-          <t>IGHV3-30-5</t>
+          <t>IGHV3-73</t>
         </is>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>IGHV3-33</t>
+          <t>IGHV3-74</t>
         </is>
       </c>
     </row>
@@ -1492,7 +1492,7 @@
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr">
         <is>
-          <t>IGHV3-43</t>
+          <t>IGHV3-9</t>
         </is>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr">
         <is>
-          <t>IGHV3-43D</t>
+          <t>IGHV4-28</t>
         </is>
       </c>
     </row>
@@ -1512,7 +1512,7 @@
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr">
         <is>
-          <t>IGHV3-48</t>
+          <t>IGHV4-30-2</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr">
         <is>
-          <t>IGHV3-49</t>
+          <t>IGHV4-30-4</t>
         </is>
       </c>
     </row>
@@ -1532,7 +1532,7 @@
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr">
         <is>
-          <t>IGHV3-53</t>
+          <t>IGHV4-31</t>
         </is>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr">
         <is>
-          <t>IGHV3-64</t>
+          <t>IGHV4-34</t>
         </is>
       </c>
     </row>
@@ -1552,7 +1552,7 @@
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>IGHV3-66</t>
+          <t>IGHV4-38-2</t>
         </is>
       </c>
     </row>
@@ -1562,7 +1562,7 @@
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
-          <t>IGHV3-7</t>
+          <t>IGHV4-39</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1572,7 @@
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
-          <t>IGHV3-72</t>
+          <t>IGHV4-4</t>
         </is>
       </c>
     </row>
@@ -1582,7 +1582,7 @@
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
-          <t>IGHV3-73</t>
+          <t>IGHV4-59</t>
         </is>
       </c>
     </row>
@@ -1592,7 +1592,7 @@
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr">
         <is>
-          <t>IGHV3-74</t>
+          <t>IGHV4-61</t>
         </is>
       </c>
     </row>
@@ -1602,7 +1602,7 @@
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr">
         <is>
-          <t>IGHV3-9</t>
+          <t>IGHV5-10-1</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1612,7 @@
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>IGHV4-28</t>
+          <t>IGHV5-51</t>
         </is>
       </c>
     </row>
@@ -1622,7 +1622,7 @@
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>IGHV4-30-2</t>
+          <t>IGHV6-1</t>
         </is>
       </c>
     </row>
@@ -1632,857 +1632,7 @@
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>IGHV4-30-4</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>IGHV4-31</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr"/>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>IGHV4-34</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr"/>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>IGHV4-38-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>IGHV4-39</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr"/>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>IGHV4-4</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr"/>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>IGHV4-59</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr"/>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>IGHV4-61</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr"/>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>IGHV5-10-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr"/>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>IGHV5-51</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr"/>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>IGHV6-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr"/>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr">
-        <is>
           <t>IGHV7-4-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr"/>
-      <c r="B63" t="inlineStr"/>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>IGKJ1</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr"/>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>IGKV1-12</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr"/>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>IGKV1-13</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr"/>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>IGKV1-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr"/>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>IGKV1-17</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr"/>
-      <c r="B68" t="inlineStr"/>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>IGKV1-27</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr"/>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>IGKV1-33</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr"/>
-      <c r="B70" t="inlineStr"/>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>IGKV1-39</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr"/>
-      <c r="B71" t="inlineStr"/>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>IGKV1-5</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr"/>
-      <c r="B72" t="inlineStr"/>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>IGKV1-6</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr"/>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>IGKV1-8</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr"/>
-      <c r="B74" t="inlineStr"/>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>IGKV1-9</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr"/>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>IGKV1D-12</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr"/>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>IGKV1D-13</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr"/>
-      <c r="B77" t="inlineStr"/>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>IGKV1D-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr"/>
-      <c r="B78" t="inlineStr"/>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>IGKV1D-17</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr"/>
-      <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>IGKV1D-33</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr"/>
-      <c r="B80" t="inlineStr"/>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>IGKV1D-39</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr"/>
-      <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>IGKV1D-43</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr"/>
-      <c r="B82" t="inlineStr"/>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>IGKV1D-8</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr"/>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>IGKV2-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr"/>
-      <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>IGKV2-28</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr"/>
-      <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>IGKV2-29</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr"/>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>IGKV2-30</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr"/>
-      <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>IGKV2-40</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr"/>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>IGKV2D-26</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr"/>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>IGKV2D-28</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr"/>
-      <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>IGKV2D-29</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr"/>
-      <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>IGKV2D-30</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr"/>
-      <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>IGKV2D-40</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr"/>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>IGKV3-11</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr"/>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>IGKV3-15</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr"/>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>IGKV3-20</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr"/>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>IGKV3D-11</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr"/>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>IGKV3D-15</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr"/>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>IGKV3D-20</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr"/>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>IGKV3D-7</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr"/>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>IGKV4-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr"/>
-      <c r="B101" t="inlineStr"/>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>IGKV5-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr"/>
-      <c r="B102" t="inlineStr"/>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>IGKV6-21</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr"/>
-      <c r="B103" t="inlineStr"/>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>IGKV6D-21</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr"/>
-      <c r="B104" t="inlineStr"/>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>IGLJ1</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr"/>
-      <c r="B105" t="inlineStr"/>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>IGLV1-36</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr"/>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>IGLV1-40</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr"/>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>IGLV1-44</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr"/>
-      <c r="B108" t="inlineStr"/>
-      <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>IGLV1-47</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr"/>
-      <c r="B109" t="inlineStr"/>
-      <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>IGLV1-51</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr"/>
-      <c r="B110" t="inlineStr"/>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>IGLV10-54</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr"/>
-      <c r="B111" t="inlineStr"/>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>IGLV2-11</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr"/>
-      <c r="B112" t="inlineStr"/>
-      <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>IGLV2-14</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr"/>
-      <c r="B113" t="inlineStr"/>
-      <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>IGLV2-18</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr"/>
-      <c r="B114" t="inlineStr"/>
-      <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>IGLV2-23</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr"/>
-      <c r="B115" t="inlineStr"/>
-      <c r="C115" t="inlineStr"/>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>IGLV2-8</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr"/>
-      <c r="B116" t="inlineStr"/>
-      <c r="C116" t="inlineStr"/>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>IGLV3-1</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr"/>
-      <c r="B117" t="inlineStr"/>
-      <c r="C117" t="inlineStr"/>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>IGLV3-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr"/>
-      <c r="B118" t="inlineStr"/>
-      <c r="C118" t="inlineStr"/>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>IGLV3-12</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr"/>
-      <c r="B119" t="inlineStr"/>
-      <c r="C119" t="inlineStr"/>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>IGLV3-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr"/>
-      <c r="B120" t="inlineStr"/>
-      <c r="C120" t="inlineStr"/>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>IGLV3-19</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr"/>
-      <c r="B121" t="inlineStr"/>
-      <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>IGLV3-21</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr"/>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" t="inlineStr"/>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>IGLV3-22</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr"/>
-      <c r="B123" t="inlineStr"/>
-      <c r="C123" t="inlineStr"/>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>IGLV3-25</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr"/>
-      <c r="B124" t="inlineStr"/>
-      <c r="C124" t="inlineStr"/>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>IGLV3-27</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr"/>
-      <c r="B125" t="inlineStr"/>
-      <c r="C125" t="inlineStr"/>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>IGLV4-3</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr"/>
-      <c r="B126" t="inlineStr"/>
-      <c r="C126" t="inlineStr"/>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>IGLV4-60</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr"/>
-      <c r="B127" t="inlineStr"/>
-      <c r="C127" t="inlineStr"/>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>IGLV4-69</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr"/>
-      <c r="B128" t="inlineStr"/>
-      <c r="C128" t="inlineStr"/>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>IGLV5-37</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr"/>
-      <c r="B129" t="inlineStr"/>
-      <c r="C129" t="inlineStr"/>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>IGLV5-39</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr"/>
-      <c r="B130" t="inlineStr"/>
-      <c r="C130" t="inlineStr"/>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>IGLV5-45</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr"/>
-      <c r="B131" t="inlineStr"/>
-      <c r="C131" t="inlineStr"/>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>IGLV5-52</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr"/>
-      <c r="B132" t="inlineStr"/>
-      <c r="C132" t="inlineStr"/>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>IGLV6-57</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr"/>
-      <c r="B133" t="inlineStr"/>
-      <c r="C133" t="inlineStr"/>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>IGLV7-43</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr"/>
-      <c r="B134" t="inlineStr"/>
-      <c r="C134" t="inlineStr"/>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>IGLV7-46</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr"/>
-      <c r="B135" t="inlineStr"/>
-      <c r="C135" t="inlineStr"/>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>IGLV8-61</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr"/>
-      <c r="B136" t="inlineStr"/>
-      <c r="C136" t="inlineStr"/>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>IGLV9-49</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Better validations for columns and blank rows
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -403,7 +403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +426,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Version 1.2.1</t>
+          <t>Version 1.2.2</t>
         </is>
       </c>
     </row>
@@ -436,95 +436,93 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Add your antibodies to the 'Antibodies' sheet. Do not edit the other sheets.</t>
+          <t>Add your antibodies to the 'Antibodies' sheet.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Do not change the headers of the 'Antibodies' sheet.</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Antibody name</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Your preferred code name for the antibody</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Host</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Specify the host species that is the source of the antibody</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Do not edit the other sheets.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Isotype</t>
+          <t>Antibody name</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Specify the antibody isotype, if known</t>
+          <t>Your preferred code name for the antibody</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Light chain</t>
+          <t>Host</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Specify the antibody light chain, if known (kappa or lambda)</t>
+          <t>Specify the host species that is the source of the antibody</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Heavy chain germline</t>
+          <t>Isotype</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Specify the antibody heavy chain germline gene, if known</t>
+          <t>Specify the antibody isotype, if known</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
+          <t>Light chain</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Specify the antibody light chain, if known (kappa or lambda)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Heavy chain germline</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Specify the antibody heavy chain germline gene, if known</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
           <t>Antibody details</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Measurements or characteristics of the antibody.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>This column is optional, and meant to capture data you might have on the antibody.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>These data will not be released to the partner reference labs that will perform the analyses.</t>
         </is>
       </c>
     </row>
@@ -532,7 +530,7 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>For example:</t>
+          <t>This column is optional, and meant to capture data you might have on the antibody.</t>
         </is>
       </c>
     </row>
@@ -540,7 +538,7 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>- Affinity: Spike protein binding affinity; inhibition of ACE2 binding; ELISA for Spike</t>
+          <t>These data will not be released to the partner reference labs that will perform the analyses.</t>
         </is>
       </c>
     </row>
@@ -548,7 +546,7 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>- Neutralization: IC50 value</t>
+          <t>For example:</t>
         </is>
       </c>
     </row>
@@ -556,7 +554,7 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>- Neutralization assay platform</t>
+          <t>- Affinity: Spike protein binding affinity; inhibition of ACE2 binding; ELISA for Spike</t>
         </is>
       </c>
     </row>
@@ -564,19 +562,15 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>- Epitope: Binning or competition data</t>
+          <t>- Neutralization: IC50 value</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Structural data</t>
-        </is>
-      </c>
+      <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Would you like structural analyses of this antibody?</t>
+          <t>- Neutralization assay platform</t>
         </is>
       </c>
     </row>
@@ -584,25 +578,45 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
+          <t>- Epitope: Binning or competition data</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Structural data</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Would you like structural analyses of this antibody?</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>If no, leave blank.</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
         <is>
           <t>If yes, rank the antibodies in order of priority, starting with '1' for the highest priority.</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
         <is>
           <t>Antibody comment</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>Please provide any other details about the antibody.</t>
         </is>

</xml_diff>

<commit_message>
Add instruction: no blank rows
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -403,7 +403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +426,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Version 1.2.2</t>
+          <t>Version 1.2.3</t>
         </is>
       </c>
     </row>
@@ -443,94 +443,93 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Do not change the headers of the 'Antibodies' sheet.</t>
+          <t>Please use consecutive rows (no blank rows).</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Do not edit the header row of the 'Antibodies' sheet.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Do not edit the other sheets.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Antibody name</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Your preferred code name for the antibody</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Host</t>
+          <t>Antibody name</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Specify the host species that is the source of the antibody</t>
+          <t>Your preferred code name for the antibody</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Isotype</t>
+          <t>Host</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Specify the antibody isotype, if known</t>
+          <t>Specify the host species that is the source of the antibody</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Light chain</t>
+          <t>Isotype</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Specify the antibody light chain, if known (kappa or lambda)</t>
+          <t>Specify the antibody isotype, if known</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Heavy chain germline</t>
+          <t>Light chain</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Specify the antibody heavy chain germline gene, if known</t>
+          <t>Specify the antibody light chain, if known (kappa or lambda)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
+          <t>Heavy chain germline</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Specify the antibody heavy chain germline gene, if known</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
           <t>Antibody details</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Measurements or characteristics of the antibody.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>This column is optional, and meant to capture data you might have on the antibody.</t>
         </is>
       </c>
     </row>
@@ -538,7 +537,7 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>These data will not be released to the partner reference labs that will perform the analyses.</t>
+          <t>This column is optional, and meant to capture data you might have on the antibody.</t>
         </is>
       </c>
     </row>
@@ -546,7 +545,7 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>For example:</t>
+          <t>These data will not be released to the partner reference labs that will perform the analyses.</t>
         </is>
       </c>
     </row>
@@ -554,7 +553,7 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>- Affinity: Spike protein binding affinity; inhibition of ACE2 binding; ELISA for Spike</t>
+          <t>For example:</t>
         </is>
       </c>
     </row>
@@ -562,7 +561,7 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>- Neutralization: IC50 value</t>
+          <t>- Affinity: Spike protein binding affinity; inhibition of ACE2 binding; ELISA for Spike</t>
         </is>
       </c>
     </row>
@@ -570,7 +569,7 @@
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>- Neutralization assay platform</t>
+          <t>- Neutralization: IC50 value</t>
         </is>
       </c>
     </row>
@@ -578,27 +577,27 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
+          <t>- Neutralization assay platform</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>- Epitope: Binning or competition data</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
         <is>
           <t>Structural data</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>Would you like structural analyses of this antibody?</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>If no, leave blank.</t>
         </is>
       </c>
     </row>
@@ -606,17 +605,25 @@
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
+          <t>If no, leave blank.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>If yes, rank the antibodies in order of priority, starting with '1' for the highest priority.</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
         <is>
           <t>Antibody comment</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>Please provide any other details about the antibody.</t>
         </is>

</xml_diff>

<commit_message>
Update hosts, add IgY
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
@@ -55,17 +55,85 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -75,37 +143,37 @@
     <author>Validation service</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Duplicate value 'VD-Crotty 1' is not allowed in column 'Antibody name'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A4" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <t>Missing required value in column 'Antibody name'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B5" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <t>Missing required value in column 'Host'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C6" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <t>'IggA1' is not a valid term in column 'Isotype'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D7" shapeId="0">
+    <comment ref="D7" authorId="0" shapeId="0">
       <text>
         <t>'kapa' is not a valid term in column 'Light chain'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E8" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <t>'IGVH1-8' is not a valid term in column 'Heavy chain germline'</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G9" shapeId="0">
+    <comment ref="G9" authorId="0" shapeId="0">
       <text>
         <t>'top' is not of type 'integer' in column 'Structural data'</t>
       </text>
@@ -411,8 +479,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="18"/>
-    <col customWidth="1" max="2" min="2" width="70"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="70" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -630,8 +698,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -644,20 +712,20 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="15"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="15"/>
-    <col customWidth="1" max="5" min="5" width="20"/>
-    <col customWidth="1" max="6" min="6" width="16"/>
-    <col customWidth="1" max="7" min="7" width="15"/>
-    <col customWidth="1" max="8" min="8" width="16"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="16" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -710,7 +778,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>human (Homo sapiens)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -744,7 +812,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>human (Homo sapiens)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -778,7 +846,7 @@
       <c r="A4" s="2" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mus musculus</t>
+          <t>mouse (Mus musculus)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -838,7 +906,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mus musculus</t>
+          <t>mouse (Mus musculus)</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -880,7 +948,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mus musculus</t>
+          <t>mouse (Mus musculus)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -910,7 +978,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>human (Homo sapiens)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -944,7 +1012,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mus musculus</t>
+          <t>mouse (Mus musculus)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -978,7 +1046,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>human (Homo sapiens)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1000,7 +1068,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mus musculus</t>
+          <t>mouse (Mus musculus)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1020,20 +1088,20 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B100" type="list">
-      <formula1>=Terminology!$A$2:$A$4</formula1>
+    <dataValidation sqref="B2:B100" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>=Terminology!$A$2:$A$6</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C100" type="list">
-      <formula1>=Terminology!$B$2:$B$15</formula1>
+    <dataValidation sqref="C2:C100" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>=Terminology!$B$2:$B$16</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D100" type="list">
+    <dataValidation sqref="D2:D100" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>=Terminology!$C$2:$C$3</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E100" type="list">
+    <dataValidation sqref="E2:E100" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>=Terminology!$D$2:$D$51</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
@@ -1047,16 +1115,16 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="15"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="20"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1084,7 +1152,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>chicken (Gallus gallus)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1106,7 +1174,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mus musculus</t>
+          <t>human (Homo sapiens)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1128,7 +1196,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mus musculus BALB/C</t>
+          <t>llama (Lama glama)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1144,7 +1212,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>mouse (Mus musculus)</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>IgD</t>
@@ -1158,7 +1230,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>alpaca (Vicugna pacos)</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>IgE</t>
@@ -1299,7 +1375,11 @@
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>IgY</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
@@ -1658,7 +1738,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change hosr sort order
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission-invalid-highlighted.xlsx
+++ b/examples/antibodies-submission-invalid-highlighted.xlsx
@@ -1152,7 +1152,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>chicken (Gallus gallus)</t>
+          <t>human (Homo sapiens)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1174,7 +1174,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>human (Homo sapiens)</t>
+          <t>mouse (Mus musculus)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1196,7 +1196,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>llama (Lama glama)</t>
+          <t>chicken (Gallus gallus)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1214,7 +1214,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>mouse (Mus musculus)</t>
+          <t>llama (Lama glama)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">

</xml_diff>